<commit_message>
- use method-name or class-name as default command-names - configuration for default command-attribute prefix
</commit_message>
<xml_diff>
--- a/examples-simple/src/test/resources/ArithmeticalTests.xlsx
+++ b/examples-simple/src/test/resources/ArithmeticalTests.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\workspace\jexunit\examples-simple\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="21315" windowHeight="10035" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="21315" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="First arithmetical Test" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="26">
   <si>
     <t>disabled</t>
   </si>
@@ -91,6 +96,9 @@
   </si>
   <si>
     <t>With a second parameter, but only one header column.</t>
+  </si>
+  <si>
+    <t>SUBTRACT</t>
   </si>
 </sst>
 </file>
@@ -159,14 +167,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -204,9 +215,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -241,7 +252,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -276,7 +287,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -452,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,7 +551,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -652,7 +663,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,7 +761,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -861,7 +872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
comment test-commands in excel file for additional info in assertions
</commit_message>
<xml_diff>
--- a/examples-simple/src/test/resources/ArithmeticalTests.xlsx
+++ b/examples-simple/src/test/resources/ArithmeticalTests.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="28">
   <si>
     <t>disabled</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>SUBTRACT</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>this should fail!</t>
   </si>
 </sst>
 </file>
@@ -461,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,7 +597,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -605,7 +611,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -619,7 +625,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -635,8 +641,11 @@
       <c r="E20" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -651,6 +660,9 @@
       </c>
       <c r="E21" t="s">
         <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>